<commit_message>
Commit casi final 3
</commit_message>
<xml_diff>
--- a/Casos de Prueba2.xlsx
+++ b/Casos de Prueba2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alero\OneDrive\Escritorio\UIS\8 OCTAVO SEMESTRE\Ingeniería del Software II\Proyecto Software\PROYECTO-SOFTWARE-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75562841-7C86-45EE-9F5C-6BB8E3D4F65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FBD38A-618F-4F94-9BEE-32563DBA1787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>Prioridad</t>
   </si>
   <si>
-    <t>Nombre del Tester</t>
-  </si>
-  <si>
     <t>Precondiciones</t>
   </si>
   <si>
@@ -76,19 +73,10 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>alta</t>
-  </si>
-  <si>
     <t>APRENDE Cómo Diseñar CASOS DE PRUEBA 🚀 (con EJEMPLOS PRÁCTICOS) - YouTube</t>
   </si>
   <si>
     <t>Verificación de pantalla inicial para cliente</t>
-  </si>
-  <si>
-    <t>media</t>
-  </si>
-  <si>
-    <t>Alejandro romero</t>
   </si>
   <si>
     <t xml:space="preserve">1. Abrir la web
@@ -105,9 +93,6 @@
 Botón carrito</t>
   </si>
   <si>
-    <t>verificar registro de usuario</t>
-  </si>
-  <si>
     <t>Dubian Palacios</t>
   </si>
   <si>
@@ -147,12 +132,27 @@
   <si>
     <t>Se muestran todos los elementos en la pantalla principal</t>
   </si>
+  <si>
+    <t>Alejandro Romero</t>
+  </si>
+  <si>
+    <t>Nombre del tester</t>
+  </si>
+  <si>
+    <t>MEDIA</t>
+  </si>
+  <si>
+    <t>ALTA</t>
+  </si>
+  <si>
+    <t>Verificar registro de usuario</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -166,15 +166,29 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -191,7 +205,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -199,30 +213,89 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,159 +516,168 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
     <col min="7" max="7" width="28.42578125" customWidth="1"/>
     <col min="8" max="8" width="45" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="174.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="8">
+      <c r="I2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="12">
         <v>44783</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="174.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="J3" s="4"/>
-      <c r="K3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" s="8">
+      <c r="K3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="5">
         <v>44784</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="174.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L4" s="8">
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="5">
         <v>44815</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>15</v>
+      <c r="A10" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -603,5 +685,6 @@
     <hyperlink ref="A10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>